<commit_message>
Added county level corrections for households by workers
</commit_message>
<xml_diff>
--- a/applications/travel_model_lu_inputs/2020/Workers/ACSPUMS_WorkerTotals_2017-2021_Comparisons.xlsx
+++ b/applications/travel_model_lu_inputs/2020/Workers/ACSPUMS_WorkerTotals_2017-2021_Comparisons.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\petrale\applications\travel_model_lu_inputs\2020\Workers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7060DF2-F62A-4E56-9707-5964EB94E91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A1AD6D-9995-456E-A343-99621FAD6F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Total Workers_21" sheetId="5" r:id="rId1"/>
-    <sheet name="Households by No. of Worker_21" sheetId="6" r:id="rId2"/>
-    <sheet name="HHs by Workers Correction_21" sheetId="7" r:id="rId3"/>
-    <sheet name="Households by No. of Worker (2)" sheetId="8" r:id="rId4"/>
+    <sheet name="Total Worker" sheetId="5" r:id="rId1"/>
+    <sheet name="Correction Factor Calcs" sheetId="6" r:id="rId2"/>
+    <sheet name="Correction Transposed" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -226,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="56">
   <si>
     <t>Alameda</t>
   </si>
@@ -346,30 +345,6 @@
   </si>
   <si>
     <t>County-Level Correction Factors for HHs by No. Workers</t>
-  </si>
-  <si>
-    <t>COUNTY_NAME</t>
-  </si>
-  <si>
-    <t>COUNTY</t>
-  </si>
-  <si>
-    <t>HH_WORKERS</t>
-  </si>
-  <si>
-    <t>CORRECTION</t>
-  </si>
-  <si>
-    <t>hh_wrks_0</t>
-  </si>
-  <si>
-    <t>hh_wrks_1</t>
-  </si>
-  <si>
-    <t>hh_wrks_2</t>
-  </si>
-  <si>
-    <t>hh_wrks_3_plus</t>
   </si>
   <si>
     <t>ACS and PUMS Data 2017-2021, and ACS 2017-2021</t>
@@ -401,41 +376,49 @@
     <t>PUMS 2017-2021 Workers (ESR==1,2,4,5), Using Person Weights</t>
   </si>
   <si>
+    <t>County_Name</t>
+  </si>
+  <si>
+    <t>Average 3+ Workers</t>
+  </si>
+  <si>
+    <t>Bay</t>
+  </si>
+  <si>
+    <t>Correction</t>
+  </si>
+  <si>
+    <t>County Code</t>
+  </si>
+  <si>
+    <t>3p</t>
+  </si>
+  <si>
     <t>ACS 2017-2021
-Refactored Using Total Worker Table (B23025) and PUMS 2017-2021</t>
-  </si>
-  <si>
-    <t>County_Name</t>
-  </si>
-  <si>
-    <t>Average 3+ Workers</t>
-  </si>
-  <si>
-    <t>Bay</t>
-  </si>
-  <si>
-    <t>Correction</t>
-  </si>
-  <si>
-    <t>County Code</t>
-  </si>
-  <si>
-    <t>3p</t>
+Values Inflated to Match Total Worker Table (B23025) from PUMS 2017-2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1072,131 +1055,127 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1521,7 +1500,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1544,7 +1523,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1557,15 +1536,15 @@
     </row>
     <row r="6" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
-      <c r="B6" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="29" t="s">
+      <c r="B6" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="28" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1585,8 +1564,8 @@
       <c r="E7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>51</v>
+      <c r="F7" s="32" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1823,10 +1802,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAACAC74-F91E-4F28-9661-7FB91FA9CF3F}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C13" sqref="C13"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1860,7 +1839,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
@@ -1871,26 +1850,26 @@
     <row r="5" spans="1:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="39" t="s">
+      <c r="C5" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="41"/>
+      <c r="G5" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="41"/>
+      <c r="I5" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="41"/>
+      <c r="K5" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" s="40"/>
+      <c r="L5" s="41"/>
       <c r="M5" s="19" t="s">
         <v>39</v>
       </c>
@@ -1926,10 +1905,10 @@
       <c r="J6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="K6" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="31" t="s">
+      <c r="L6" s="30" t="s">
         <v>29</v>
       </c>
       <c r="M6" s="8" t="s">
@@ -1950,7 +1929,7 @@
         <f>0*C7</f>
         <v>0</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="20">
         <v>132234</v>
       </c>
       <c r="F7" s="15">
@@ -1972,24 +1951,24 @@
         <f>0*I7</f>
         <v>0</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="20">
         <f>K11-SUM(K8:K10)</f>
         <v>78056.507639411371</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="21">
         <f>J7*$L$11/$J$11</f>
         <v>0</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="23">
         <f>K7/E7</f>
         <v>0.59029075456699009</v>
       </c>
       <c r="N7" s="15"/>
-      <c r="O7" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="P7" s="35" t="s">
-        <v>59</v>
+      <c r="O7" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" s="34" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
@@ -2032,15 +2011,15 @@
         <f>J8*$L$11/$J$11</f>
         <v>227221.37125646483</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="24">
         <f t="shared" ref="M8:M56" si="0">K8/E8</f>
         <v>1.0654264646194687</v>
       </c>
       <c r="N8" s="15"/>
-      <c r="O8" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="P8" s="34">
+      <c r="O8" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" s="33">
         <v>3.4198110000679902</v>
       </c>
     </row>
@@ -2084,15 +2063,15 @@
         <f>J9*$L$11/$J$11</f>
         <v>417636.77682349941</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="24">
         <f t="shared" si="0"/>
         <v>1.1410529133725837</v>
       </c>
       <c r="N9" s="15"/>
-      <c r="O9" s="34" t="s">
+      <c r="O9" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="P9" s="34">
+      <c r="P9" s="33">
         <v>3.3412041935173602</v>
       </c>
     </row>
@@ -2137,15 +2116,15 @@
         <f>J10*$L$11/$J$11</f>
         <v>231133.85192003576</v>
       </c>
-      <c r="M10" s="26">
+      <c r="M10" s="25">
         <f t="shared" si="0"/>
         <v>1.2710006900175661</v>
       </c>
       <c r="N10" s="15"/>
-      <c r="O10" s="34" t="s">
+      <c r="O10" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="34">
+      <c r="P10" s="33">
         <v>3.30607548327708</v>
       </c>
     </row>
@@ -2193,15 +2172,15 @@
       <c r="L11" s="14">
         <v>875992</v>
       </c>
-      <c r="M11" s="27">
+      <c r="M11" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N11" s="15"/>
-      <c r="O11" s="34" t="s">
+      <c r="O11" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="P11" s="34">
+      <c r="P11" s="33">
         <v>3.4015181781861799</v>
       </c>
     </row>
@@ -2249,15 +2228,15 @@
         <f>J12*$L$16/$J$16</f>
         <v>0</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="24">
         <f>K12/E12</f>
         <v>0.80717875648182613</v>
       </c>
       <c r="N12" s="15"/>
-      <c r="O12" s="34" t="s">
+      <c r="O12" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="P12" s="34">
+      <c r="P12" s="33">
         <v>3.50347024006249</v>
       </c>
     </row>
@@ -2301,15 +2280,15 @@
         <f>J13*$L$16/$J$16</f>
         <v>150234.70583864287</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="24">
         <f t="shared" si="0"/>
         <v>1.0189479577501703</v>
       </c>
       <c r="N13" s="15"/>
-      <c r="O13" s="34" t="s">
+      <c r="O13" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="P13" s="34">
+      <c r="P13" s="33">
         <v>3.4803882462438498</v>
       </c>
     </row>
@@ -2353,15 +2332,15 @@
         <f>J14*$L$16/$J$16</f>
         <v>268019.06836255552</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="24">
         <f t="shared" si="0"/>
         <v>1.0706972154367396</v>
       </c>
       <c r="N14" s="15"/>
-      <c r="O14" s="34" t="s">
+      <c r="O14" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="P14" s="34">
+      <c r="P14" s="33">
         <v>3.4814628223014501</v>
       </c>
     </row>
@@ -2406,15 +2385,15 @@
         <f>J15*$L$16/$J$16</f>
         <v>152859.22579880161</v>
       </c>
-      <c r="M15" s="26">
+      <c r="M15" s="25">
         <f t="shared" si="0"/>
         <v>1.1597186442156466</v>
       </c>
       <c r="N15" s="15"/>
-      <c r="O15" s="34" t="s">
+      <c r="O15" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="34">
+      <c r="P15" s="33">
         <v>3.3654663518299901</v>
       </c>
     </row>
@@ -2462,15 +2441,15 @@
       <c r="L16" s="14">
         <v>571113</v>
       </c>
-      <c r="M16" s="27">
+      <c r="M16" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N16" s="15"/>
-      <c r="O16" s="34" t="s">
+      <c r="O16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P16" s="34">
+      <c r="P16" s="33">
         <v>3.3988417199366201</v>
       </c>
     </row>
@@ -2518,15 +2497,15 @@
         <f>J17*$L$21/$J$21</f>
         <v>0</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="24">
         <f>K17/E17</f>
         <v>0.81702218159322271</v>
       </c>
       <c r="N17" s="15"/>
-      <c r="O17" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="P17" s="34">
+      <c r="O17" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="P17" s="33">
         <v>3.4336076674653602</v>
       </c>
     </row>
@@ -2570,7 +2549,7 @@
         <f>J18*$L$21/$J$21</f>
         <v>40586.456348778876</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="24">
         <f t="shared" si="0"/>
         <v>1.0572693640923954</v>
       </c>
@@ -2616,7 +2595,7 @@
         <f>J19*$L$21/$J$21</f>
         <v>66038.007817669786</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="24">
         <f t="shared" si="0"/>
         <v>1.0655072415642612</v>
       </c>
@@ -2664,7 +2643,7 @@
         <f>J20*$L$21/$J$21</f>
         <v>24131.535833551345</v>
       </c>
-      <c r="M20" s="26">
+      <c r="M20" s="25">
         <f t="shared" si="0"/>
         <v>1.1385350925744731</v>
       </c>
@@ -2714,7 +2693,7 @@
       <c r="L21" s="14">
         <v>130756</v>
       </c>
-      <c r="M21" s="27">
+      <c r="M21" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2764,7 +2743,7 @@
         <f>J22*$L$26/$J$26</f>
         <v>0</v>
       </c>
-      <c r="M22" s="25">
+      <c r="M22" s="24">
         <f>K22/E22</f>
         <v>0.70343787377412059</v>
       </c>
@@ -2810,7 +2789,7 @@
         <f>J23*$L$26/$J$26</f>
         <v>17932.399304007708</v>
       </c>
-      <c r="M23" s="25">
+      <c r="M23" s="24">
         <f t="shared" si="0"/>
         <v>1.0919741385950377</v>
       </c>
@@ -2856,7 +2835,7 @@
         <f>J24*$L$26/$J$26</f>
         <v>32128.671718842121</v>
       </c>
-      <c r="M24" s="25">
+      <c r="M24" s="24">
         <f t="shared" si="0"/>
         <v>1.0863088896010995</v>
       </c>
@@ -2903,7 +2882,7 @@
         <f>J25*$L$26/$J$26</f>
         <v>20158.928977150172</v>
       </c>
-      <c r="M25" s="26">
+      <c r="M25" s="25">
         <f t="shared" si="0"/>
         <v>1.1867141492931483</v>
       </c>
@@ -2953,7 +2932,7 @@
       <c r="L26" s="14">
         <v>70220</v>
       </c>
-      <c r="M26" s="27">
+      <c r="M26" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3003,7 +2982,7 @@
         <f>J27*$L$31/$J$31</f>
         <v>0</v>
       </c>
-      <c r="M27" s="25">
+      <c r="M27" s="24">
         <f>K27/E27</f>
         <v>0.75146859073490047</v>
       </c>
@@ -3049,7 +3028,7 @@
         <f>J28*$L$31/$J$31</f>
         <v>144381.76648931694</v>
       </c>
-      <c r="M28" s="25">
+      <c r="M28" s="24">
         <f t="shared" si="0"/>
         <v>1.0536430916312145</v>
       </c>
@@ -3095,7 +3074,7 @@
         <f>J29*$L$31/$J$31</f>
         <v>234722.72435783289</v>
       </c>
-      <c r="M29" s="25">
+      <c r="M29" s="24">
         <f t="shared" si="0"/>
         <v>1.0634218497210675</v>
       </c>
@@ -3142,7 +3121,7 @@
         <f>J30*$L$31/$J$31</f>
         <v>133083.50915285017</v>
       </c>
-      <c r="M30" s="26">
+      <c r="M30" s="25">
         <f t="shared" si="0"/>
         <v>1.1871057393021571</v>
       </c>
@@ -3192,7 +3171,7 @@
       <c r="L31" s="14">
         <v>512188</v>
       </c>
-      <c r="M31" s="27">
+      <c r="M31" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3242,7 +3221,7 @@
         <f>J32*$L$36/$J$36</f>
         <v>0</v>
       </c>
-      <c r="M32" s="25">
+      <c r="M32" s="24">
         <f>K32/E32</f>
         <v>0.74298739554270166</v>
       </c>
@@ -3288,7 +3267,7 @@
         <f>J33*$L$36/$J$36</f>
         <v>93659.546667607327</v>
       </c>
-      <c r="M33" s="25">
+      <c r="M33" s="24">
         <f t="shared" si="0"/>
         <v>1.02063451242952</v>
       </c>
@@ -3334,7 +3313,7 @@
         <f>J34*$L$36/$J$36</f>
         <v>198449.17134891596</v>
       </c>
-      <c r="M34" s="25">
+      <c r="M34" s="24">
         <f t="shared" si="0"/>
         <v>1.063557379006999</v>
       </c>
@@ -3381,7 +3360,7 @@
         <f>J35*$L$36/$J$36</f>
         <v>117698.2819834767</v>
       </c>
-      <c r="M35" s="26">
+      <c r="M35" s="25">
         <f t="shared" si="0"/>
         <v>1.1895030791292394</v>
       </c>
@@ -3431,7 +3410,7 @@
       <c r="L36" s="14">
         <v>409807</v>
       </c>
-      <c r="M36" s="27">
+      <c r="M36" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3481,7 +3460,7 @@
         <f>J37*$L$41/$J$41</f>
         <v>0</v>
       </c>
-      <c r="M37" s="25">
+      <c r="M37" s="24">
         <f>K37/E37</f>
         <v>0.6887759307446365</v>
       </c>
@@ -3527,7 +3506,7 @@
         <f>J38*$L$41/$J$41</f>
         <v>250590.25336944056</v>
       </c>
-      <c r="M38" s="25">
+      <c r="M38" s="24">
         <f t="shared" si="0"/>
         <v>1.0483368754892173</v>
       </c>
@@ -3573,7 +3552,7 @@
         <f>J39*$L$41/$J$41</f>
         <v>464073.99039200199</v>
       </c>
-      <c r="M39" s="25">
+      <c r="M39" s="24">
         <f t="shared" si="0"/>
         <v>1.0594135583132487</v>
       </c>
@@ -3620,7 +3599,7 @@
         <f>J40*$L$41/$J$41</f>
         <v>294332.75623855746</v>
       </c>
-      <c r="M40" s="26">
+      <c r="M40" s="25">
         <f t="shared" si="0"/>
         <v>1.1564102497941353</v>
       </c>
@@ -3670,7 +3649,7 @@
       <c r="L41" s="14">
         <v>1008997</v>
       </c>
-      <c r="M41" s="27">
+      <c r="M41" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3720,7 +3699,7 @@
         <f>J42*$L$46/$J$46</f>
         <v>0</v>
       </c>
-      <c r="M42" s="25">
+      <c r="M42" s="24">
         <f>K42/E42</f>
         <v>0.79449824296187188</v>
       </c>
@@ -3766,7 +3745,7 @@
         <f>J43*$L$46/$J$46</f>
         <v>58740.639270258172</v>
       </c>
-      <c r="M43" s="25">
+      <c r="M43" s="24">
         <f t="shared" si="0"/>
         <v>1.0232669500959528</v>
       </c>
@@ -3812,7 +3791,7 @@
         <f>J44*$L$46/$J$46</f>
         <v>95696.643877779439</v>
       </c>
-      <c r="M44" s="25">
+      <c r="M44" s="24">
         <f t="shared" si="0"/>
         <v>1.0658778360671342</v>
       </c>
@@ -3859,7 +3838,7 @@
         <f>J45*$L$46/$J$46</f>
         <v>61867.716851962396</v>
       </c>
-      <c r="M45" s="26">
+      <c r="M45" s="25">
         <f t="shared" si="0"/>
         <v>1.2044227001564902</v>
       </c>
@@ -3909,7 +3888,7 @@
       <c r="L46" s="14">
         <v>216305</v>
       </c>
-      <c r="M46" s="27">
+      <c r="M46" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3959,7 +3938,7 @@
         <f>J47*$L$51/$J$51</f>
         <v>0</v>
       </c>
-      <c r="M47" s="25">
+      <c r="M47" s="24">
         <f>K47/E47</f>
         <v>0.83816909998828981</v>
       </c>
@@ -4005,7 +3984,7 @@
         <f>J48*$L$51/$J$51</f>
         <v>66857.954672067877</v>
       </c>
-      <c r="M48" s="25">
+      <c r="M48" s="24">
         <f t="shared" si="0"/>
         <v>1.0308041115027424</v>
       </c>
@@ -4051,7 +4030,7 @@
         <f>J49*$L$51/$J$51</f>
         <v>116840.15702222823</v>
       </c>
-      <c r="M49" s="25">
+      <c r="M49" s="24">
         <f t="shared" si="0"/>
         <v>1.0827355347155851</v>
       </c>
@@ -4098,7 +4077,7 @@
         <f>J50*$L$51/$J$51</f>
         <v>68406.888305703891</v>
       </c>
-      <c r="M50" s="26">
+      <c r="M50" s="25">
         <f t="shared" si="0"/>
         <v>1.1057317628900591</v>
       </c>
@@ -4148,7 +4127,7 @@
       <c r="L51" s="14">
         <v>252105</v>
       </c>
-      <c r="M51" s="27">
+      <c r="M51" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4193,7 +4172,7 @@
         <f t="shared" ref="J52:L55" si="11">J7+J12+J17+J22+J27+J32+J37+J42+J47</f>
         <v>0</v>
       </c>
-      <c r="K52" s="23">
+      <c r="K52" s="22">
         <f t="shared" si="11"/>
         <v>436292.98564051313</v>
       </c>
@@ -4201,7 +4180,7 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M52" s="28">
+      <c r="M52" s="27">
         <f>K52/E52</f>
         <v>0.72401876810368604</v>
       </c>
@@ -4251,7 +4230,7 @@
         <f t="shared" si="11"/>
         <v>1050205.093216585</v>
       </c>
-      <c r="M53" s="25">
+      <c r="M53" s="24">
         <f t="shared" si="0"/>
         <v>1.044339040824275</v>
       </c>
@@ -4301,7 +4280,7 @@
         <f t="shared" si="11"/>
         <v>1893605.2117213253</v>
       </c>
-      <c r="M54" s="25">
+      <c r="M54" s="24">
         <f t="shared" si="0"/>
         <v>1.0814779768383678</v>
       </c>
@@ -4352,7 +4331,7 @@
         <f>L10+L15+L20+L25+L30+L35+L40+L45+L50</f>
         <v>1103672.6950620897</v>
       </c>
-      <c r="M55" s="26">
+      <c r="M55" s="25">
         <f t="shared" si="0"/>
         <v>1.1859054107346698</v>
       </c>
@@ -4403,7 +4382,7 @@
         <f>SUM(L52:L55)</f>
         <v>4047483</v>
       </c>
-      <c r="M56" s="27">
+      <c r="M56" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4424,551 +4403,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB135DF-2D59-4A10-9446-A7E0B5ED4BCE}">
-  <dimension ref="A1:D37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="14.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.7243926284066956</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.71045461057797943</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.65234440973873298</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.61093155138835786</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.81432449606111224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.79221032005758307</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.71025600208376349</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.81645903954103427</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.81952491588983412</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1.0549854708758115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1.0162564381618149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1.0467479421237909</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1">
-        <v>4</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1.0636388531450143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1.0207878838846087</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="1">
-        <v>6</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1.0348733305007278</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="1">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1.0667906227589079</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="1">
-        <v>8</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1.0465230399958017</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1">
-        <v>9</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1.0466453858424083</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1.077399993791341</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1">
-        <v>2</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1.080655652908822</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1.0807546811717326</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="1">
-        <v>4</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1.1506869686500032</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="1">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1.0761103527203895</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="1">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1.1032421402931711</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="1">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1.0848258755408788</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="1">
-        <v>8</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1.0691305300394971</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="1">
-        <v>9</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1.0649963701049894</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1.2175676189166291</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1">
-        <v>2</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1.2111886446550346</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="1">
-        <v>3</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1.2047919789524975</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1">
-        <v>4</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1.3420147906012951</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="1">
-        <v>5</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1.1536676698765049</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="1">
-        <v>6</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1.1188919031557478</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="1">
-        <v>7</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1.2652338137782535</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="1">
-        <v>8</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1.1597473621148717</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="1">
-        <v>9</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1.1826070606325927</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{744BAB6F-722F-493E-8011-419B0C28660E}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4977,657 +4416,684 @@
     <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.58203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="4.9140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.58203125" style="1" customWidth="1"/>
+    <col min="6" max="14" width="6.75" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>62</v>
+      <c r="C1" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="36">
         <v>0.75146859073490047</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2" s="15">
         <v>1</v>
       </c>
-      <c r="E2" s="35">
-        <v>0</v>
-      </c>
-      <c r="F2" s="44">
+      <c r="E2" s="34">
+        <v>0</v>
+      </c>
+      <c r="F2" s="43">
         <v>0.75146859073490047</v>
       </c>
-      <c r="G2" s="44">
+      <c r="G2" s="43">
         <v>0.74298739554270166</v>
       </c>
-      <c r="H2" s="44">
+      <c r="H2" s="43">
         <v>0.6887759307446365</v>
       </c>
-      <c r="I2" s="44">
+      <c r="I2" s="43">
         <v>0.59029075456699009</v>
       </c>
-      <c r="J2" s="44">
+      <c r="J2" s="43">
         <v>0.80717875648182613</v>
       </c>
-      <c r="K2" s="44">
+      <c r="K2" s="43">
         <v>0.79449824296187188</v>
       </c>
-      <c r="L2" s="44">
+      <c r="L2" s="43">
         <v>0.70343787377412059</v>
       </c>
-      <c r="M2" s="44">
+      <c r="M2" s="43">
         <v>0.83816909998828981</v>
       </c>
-      <c r="N2" s="44">
+      <c r="N2" s="43">
         <v>0.81702218159322271</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="36">
         <v>0.74298739554270166</v>
       </c>
-      <c r="D3" s="45">
+      <c r="D3" s="15">
         <v>2</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="34">
         <v>1</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="43">
         <v>1.0536430916312145</v>
       </c>
-      <c r="G3" s="44">
+      <c r="G3" s="43">
         <v>1.02063451242952</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="43">
         <v>1.0483368754892173</v>
       </c>
-      <c r="I3" s="44">
+      <c r="I3" s="43">
         <v>1.0654264646194687</v>
       </c>
-      <c r="J3" s="44">
+      <c r="J3" s="43">
         <v>1.0189479577501703</v>
       </c>
-      <c r="K3" s="44">
+      <c r="K3" s="43">
         <v>1.0232669500959528</v>
       </c>
-      <c r="L3" s="44">
+      <c r="L3" s="43">
         <v>1.0919741385950377</v>
       </c>
-      <c r="M3" s="44">
+      <c r="M3" s="43">
         <v>1.0308041115027424</v>
       </c>
-      <c r="N3" s="44">
+      <c r="N3" s="43">
         <v>1.0572693640923954</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="36">
         <v>0.6887759307446365</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="15">
         <v>3</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="34">
         <v>2</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="43">
         <v>1.0634218497210675</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="43">
         <v>1.063557379006999</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="43">
         <v>1.0594135583132487</v>
       </c>
-      <c r="I4" s="44">
+      <c r="I4" s="43">
         <v>1.1410529133725837</v>
       </c>
-      <c r="J4" s="44">
+      <c r="J4" s="43">
         <v>1.0706972154367396</v>
       </c>
-      <c r="K4" s="44">
+      <c r="K4" s="43">
         <v>1.0658778360671342</v>
       </c>
-      <c r="L4" s="44">
+      <c r="L4" s="43">
         <v>1.0863088896010995</v>
       </c>
-      <c r="M4" s="44">
+      <c r="M4" s="43">
         <v>1.0827355347155851</v>
       </c>
-      <c r="N4" s="44">
+      <c r="N4" s="43">
         <v>1.0655072415642612</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="42" t="s">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="36">
         <v>0.59029075456699009</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="15">
         <v>4</v>
       </c>
-      <c r="E5" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="44">
+      <c r="E5" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="43">
         <v>1.1871057393021571</v>
       </c>
-      <c r="G5" s="44">
+      <c r="G5" s="43">
         <v>1.1895030791292394</v>
       </c>
-      <c r="H5" s="44">
+      <c r="H5" s="43">
         <v>1.1564102497941353</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="43">
         <v>1.2710006900175661</v>
       </c>
-      <c r="J5" s="44">
+      <c r="J5" s="43">
         <v>1.1597186442156466</v>
       </c>
-      <c r="K5" s="44">
+      <c r="K5" s="43">
         <v>1.2044227001564902</v>
       </c>
-      <c r="L5" s="44">
+      <c r="L5" s="43">
         <v>1.1867141492931483</v>
       </c>
-      <c r="M5" s="44">
+      <c r="M5" s="43">
         <v>1.1057317628900591</v>
       </c>
-      <c r="N5" s="44">
+      <c r="N5" s="43">
         <v>1.1385350925744731</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="36">
         <v>0.80717875648182613</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="15">
         <v>5</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="36">
         <v>0.79449824296187188</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="15">
         <v>6</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="36">
         <v>0.70343787377412059</v>
       </c>
-      <c r="D8" s="45">
+      <c r="D8" s="15">
         <v>7</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="36">
         <v>0.83816909998828981</v>
       </c>
-      <c r="D9" s="45">
+      <c r="D9" s="15">
         <v>8</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="36">
         <v>0.81702218159322271</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="15">
         <v>9</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="36">
         <v>1.0536430916312145</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="36">
         <v>1.02063451242952</v>
       </c>
-      <c r="D12" s="45">
+      <c r="D12" s="15">
         <v>2</v>
       </c>
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="36">
         <v>1.0483368754892173</v>
       </c>
-      <c r="D13" s="45">
+      <c r="D13" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="42" t="s">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="36">
         <v>1.0654264646194687</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D14" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="44">
+      <c r="C15" s="36">
         <v>1.0189479577501703</v>
       </c>
-      <c r="D15" s="45">
+      <c r="D15" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="36">
         <v>1.0232669500959528</v>
       </c>
-      <c r="D16" s="45">
+      <c r="D16" s="15">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="36">
         <v>1.0919741385950377</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="15">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="36">
         <v>1.0308041115027424</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D18" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C19" s="36">
         <v>1.0572693640923954</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D19" s="15">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="36">
         <v>1.0634218497210675</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="44">
+      <c r="C21" s="36">
         <v>1.063557379006999</v>
       </c>
-      <c r="D21" s="45">
+      <c r="D21" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="44">
+      <c r="C22" s="36">
         <v>1.0594135583132487</v>
       </c>
-      <c r="D22" s="45">
+      <c r="D22" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="42" t="s">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="44">
+      <c r="C23" s="36">
         <v>1.1410529133725837</v>
       </c>
-      <c r="D23" s="45">
+      <c r="D23" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="44">
+      <c r="C24" s="36">
         <v>1.0706972154367396</v>
       </c>
-      <c r="D24" s="45">
+      <c r="D24" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="44">
+      <c r="C25" s="36">
         <v>1.0658778360671342</v>
       </c>
-      <c r="D25" s="45">
+      <c r="D25" s="15">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="44">
+      <c r="C26" s="36">
         <v>1.0863088896010995</v>
       </c>
-      <c r="D26" s="45">
+      <c r="D26" s="15">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="44">
+      <c r="C27" s="36">
         <v>1.0827355347155851</v>
       </c>
-      <c r="D27" s="45">
+      <c r="D27" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="44">
+      <c r="C28" s="36">
         <v>1.0655072415642612</v>
       </c>
-      <c r="D28" s="45">
+      <c r="D28" s="15">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="44">
+      <c r="C29" s="36">
         <v>1.1871057393021571</v>
       </c>
-      <c r="D29" s="45">
+      <c r="D29" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="44">
+      <c r="C30" s="36">
         <v>1.1895030791292394</v>
       </c>
-      <c r="D30" s="45">
+      <c r="D30" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="44">
+      <c r="C31" s="36">
         <v>1.1564102497941353</v>
       </c>
-      <c r="D31" s="45">
+      <c r="D31" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="42" t="s">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="44">
+      <c r="C32" s="36">
         <v>1.2710006900175661</v>
       </c>
-      <c r="D32" s="45">
+      <c r="D32" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="44">
+      <c r="C33" s="36">
         <v>1.1597186442156466</v>
       </c>
-      <c r="D33" s="45">
+      <c r="D33" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="44">
+      <c r="C34" s="36">
         <v>1.2044227001564902</v>
       </c>
-      <c r="D34" s="45">
+      <c r="D34" s="15">
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="44">
+      <c r="C35" s="36">
         <v>1.1867141492931483</v>
       </c>
-      <c r="D35" s="45">
+      <c r="D35" s="15">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="44">
+      <c r="C36" s="36">
         <v>1.1057317628900591</v>
       </c>
-      <c r="D36" s="45">
+      <c r="D36" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="44">
+      <c r="C37" s="36">
         <v>1.1385350925744731</v>
       </c>
-      <c r="D37" s="45">
+      <c r="D37" s="15">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated calculations for empres variable and occupations
Scaled empres to county with an "2020" value (calculated from averaging 2019 and 2021 values).
</commit_message>
<xml_diff>
--- a/applications/travel_model_lu_inputs/2020/Workers/ACSPUMS_WorkerTotals_2017-2021_Comparisons.xlsx
+++ b/applications/travel_model_lu_inputs/2020/Workers/ACSPUMS_WorkerTotals_2017-2021_Comparisons.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\petrale\applications\travel_model_lu_inputs\2020\Workers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A1AD6D-9995-456E-A343-99621FAD6F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB2225E-7D42-4720-B748-2BB841EFF449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Worker" sheetId="5" r:id="rId1"/>
     <sheet name="Correction Factor Calcs" sheetId="6" r:id="rId2"/>
     <sheet name="Correction Transposed" sheetId="8" r:id="rId3"/>
+    <sheet name="ACS 2017-2021 B23025" sheetId="9" r:id="rId4"/>
+    <sheet name="ACS 2019 B23025" sheetId="10" r:id="rId5"/>
+    <sheet name="ACS 2021 B23025" sheetId="11" r:id="rId6"/>
+    <sheet name="Avg. ACS 2019 and 2021 B23025" sheetId="12" r:id="rId7"/>
+    <sheet name="Ratio 19_21 Avg. to 17-21 total" sheetId="13" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -220,12 +225,228 @@
         </r>
       </text>
     </comment>
+    <comment ref="L16" authorId="0" shapeId="0" xr:uid="{398A1039-DDCD-48D0-9345-E0A86DC0D1A4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shimon Israel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These county worker totals come from Table B23025.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L21" authorId="0" shapeId="0" xr:uid="{89ACDE23-4B1E-4557-B5DA-289461A6CD77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shimon Israel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These county worker totals come from Table B23025.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L26" authorId="0" shapeId="0" xr:uid="{C6FBD2AA-6B1A-4F98-B45A-18F07835516A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shimon Israel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These county worker totals come from Table B23025.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L31" authorId="0" shapeId="0" xr:uid="{0C3FBBCA-ACA8-47CC-8320-53464B546CCA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shimon Israel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These county worker totals come from Table B23025.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L36" authorId="0" shapeId="0" xr:uid="{BEF4448E-66BF-4A88-91DD-24C46CB55FC7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shimon Israel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These county worker totals come from Table B23025.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L41" authorId="0" shapeId="0" xr:uid="{559C10E6-9657-4A5C-ADFE-C81186BAA008}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shimon Israel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These county worker totals come from Table B23025.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L46" authorId="0" shapeId="0" xr:uid="{01EFD81E-65F0-4741-9770-A4025AD76B08}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shimon Israel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These county worker totals come from Table B23025.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L51" authorId="0" shapeId="0" xr:uid="{7CE658F5-950B-4769-8F5F-15569C1AE35B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shimon Israel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These county worker totals come from Table B23025.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L56" authorId="0" shapeId="0" xr:uid="{C0D41F99-3E42-4951-B91E-5868C3726607}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shimon Israel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These county worker totals come from Table B23025.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="89">
   <si>
     <t>Alameda</t>
   </si>
@@ -396,15 +617,115 @@
   <si>
     <t>ACS 2017-2021
 Values Inflated to Match Total Worker Table (B23025) from PUMS 2017-2021</t>
+  </si>
+  <si>
+    <t>Label (Grouping)</t>
+  </si>
+  <si>
+    <t>Alameda County, California!!Estimate</t>
+  </si>
+  <si>
+    <t>Contra Costa County, California!!Estimate</t>
+  </si>
+  <si>
+    <t>Marin County, California!!Estimate</t>
+  </si>
+  <si>
+    <t>Napa County, California!!Estimate</t>
+  </si>
+  <si>
+    <t>San Francisco County, California!!Estimate</t>
+  </si>
+  <si>
+    <t>San Mateo County, California!!Estimate</t>
+  </si>
+  <si>
+    <t>Santa Clara County, California!!Estimate</t>
+  </si>
+  <si>
+    <t>Solano County, California!!Estimate</t>
+  </si>
+  <si>
+    <t>Sonoma County, California!!Estimate</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>    In labor force:</t>
+  </si>
+  <si>
+    <t>        Civilian labor force:</t>
+  </si>
+  <si>
+    <t>            Employed</t>
+  </si>
+  <si>
+    <t>            Unemployed</t>
+  </si>
+  <si>
+    <t>        Armed Forces</t>
+  </si>
+  <si>
+    <t>    Not in labor force</t>
+  </si>
+  <si>
+    <t>ACS 2017-2021 Table B23025</t>
+  </si>
+  <si>
+    <t>ACS 2019 Table B23025</t>
+  </si>
+  <si>
+    <t>Total (civilian employed+armed forces)</t>
+  </si>
+  <si>
+    <t>Average of ACS 2019 and ACS 2021 Table B23025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alameda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contra Costa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Francisco </t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Mateo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa Clara </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solano </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonoma </t>
+  </si>
+  <si>
+    <t>Average 2019/2021 1-Year</t>
+  </si>
+  <si>
+    <t>2017-2021 5-year</t>
+  </si>
+  <si>
+    <t>Ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -1097,7 +1418,7 @@
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1157,6 +1478,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1175,7 +1497,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1499,7 +1827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071580FC-CDD4-4AB0-914B-F1C14989D30E}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1536,11 +1864,11 @@
     </row>
     <row r="6" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="31" t="s">
         <v>42</v>
       </c>
@@ -1802,10 +2130,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAACAC74-F91E-4F28-9661-7FB91FA9CF3F}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C13" sqref="C13"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1850,26 +2178,26 @@
     <row r="5" spans="1:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="40" t="s">
+      <c r="D5" s="40"/>
+      <c r="E5" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="40" t="s">
+      <c r="F5" s="42"/>
+      <c r="G5" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="40" t="s">
+      <c r="H5" s="42"/>
+      <c r="I5" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="41"/>
-      <c r="K5" s="42" t="s">
+      <c r="J5" s="42"/>
+      <c r="K5" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="41"/>
+      <c r="L5" s="42"/>
       <c r="M5" s="19" t="s">
         <v>39</v>
       </c>
@@ -2170,6 +2498,7 @@
         <v>581683</v>
       </c>
       <c r="L11" s="14">
+        <f>'ACS 2017-2021 B23025'!B$11</f>
         <v>875992</v>
       </c>
       <c r="M11" s="26">
@@ -2439,6 +2768,7 @@
         <v>405106</v>
       </c>
       <c r="L16" s="14">
+        <f>'ACS 2017-2021 B23025'!C$11</f>
         <v>571113</v>
       </c>
       <c r="M16" s="26">
@@ -2691,6 +3021,7 @@
         <v>103751</v>
       </c>
       <c r="L21" s="14">
+        <f>'ACS 2017-2021 B23025'!D$11</f>
         <v>130756</v>
       </c>
       <c r="M21" s="26">
@@ -2794,6 +3125,7 @@
         <v>1.0919741385950377</v>
       </c>
       <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
@@ -2930,6 +3262,7 @@
         <v>48745</v>
       </c>
       <c r="L26" s="14">
+        <f>'ACS 2017-2021 B23025'!E$11</f>
         <v>70220</v>
       </c>
       <c r="M26" s="26">
@@ -3169,6 +3502,7 @@
         <v>361222</v>
       </c>
       <c r="L31" s="14">
+        <f>'ACS 2017-2021 B23025'!F$11</f>
         <v>512188</v>
       </c>
       <c r="M31" s="26">
@@ -3408,6 +3742,7 @@
         <v>264892</v>
       </c>
       <c r="L36" s="14">
+        <f>'ACS 2017-2021 B23025'!G$11</f>
         <v>409807</v>
       </c>
       <c r="M36" s="26">
@@ -3647,6 +3982,7 @@
         <v>646847</v>
       </c>
       <c r="L41" s="14">
+        <f>'ACS 2017-2021 B23025'!H$11</f>
         <v>1008997</v>
       </c>
       <c r="M41" s="26">
@@ -3886,6 +4222,7 @@
         <v>153632</v>
       </c>
       <c r="L46" s="14">
+        <f>'ACS 2017-2021 B23025'!I$11</f>
         <v>216305</v>
       </c>
       <c r="M46" s="26">
@@ -4125,6 +4462,7 @@
         <v>188841</v>
       </c>
       <c r="L51" s="14">
+        <f>'ACS 2017-2021 B23025'!J$11</f>
         <v>252105</v>
       </c>
       <c r="M51" s="26">
@@ -4379,7 +4717,7 @@
         <v>2754719</v>
       </c>
       <c r="L56" s="14">
-        <f>SUM(L52:L55)</f>
+        <f>'ACS 2017-2021 B23025'!K$11</f>
         <v>4047483</v>
       </c>
       <c r="M56" s="26">
@@ -4478,31 +4816,31 @@
       <c r="E2" s="34">
         <v>0</v>
       </c>
-      <c r="F2" s="43">
+      <c r="F2" s="37">
         <v>0.75146859073490047</v>
       </c>
-      <c r="G2" s="43">
+      <c r="G2" s="37">
         <v>0.74298739554270166</v>
       </c>
-      <c r="H2" s="43">
+      <c r="H2" s="37">
         <v>0.6887759307446365</v>
       </c>
-      <c r="I2" s="43">
+      <c r="I2" s="37">
         <v>0.59029075456699009</v>
       </c>
-      <c r="J2" s="43">
+      <c r="J2" s="37">
         <v>0.80717875648182613</v>
       </c>
-      <c r="K2" s="43">
+      <c r="K2" s="37">
         <v>0.79449824296187188</v>
       </c>
-      <c r="L2" s="43">
+      <c r="L2" s="37">
         <v>0.70343787377412059</v>
       </c>
-      <c r="M2" s="43">
+      <c r="M2" s="37">
         <v>0.83816909998828981</v>
       </c>
-      <c r="N2" s="43">
+      <c r="N2" s="37">
         <v>0.81702218159322271</v>
       </c>
     </row>
@@ -4522,31 +4860,31 @@
       <c r="E3" s="34">
         <v>1</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="37">
         <v>1.0536430916312145</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="37">
         <v>1.02063451242952</v>
       </c>
-      <c r="H3" s="43">
+      <c r="H3" s="37">
         <v>1.0483368754892173</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="37">
         <v>1.0654264646194687</v>
       </c>
-      <c r="J3" s="43">
+      <c r="J3" s="37">
         <v>1.0189479577501703</v>
       </c>
-      <c r="K3" s="43">
+      <c r="K3" s="37">
         <v>1.0232669500959528</v>
       </c>
-      <c r="L3" s="43">
+      <c r="L3" s="37">
         <v>1.0919741385950377</v>
       </c>
-      <c r="M3" s="43">
+      <c r="M3" s="37">
         <v>1.0308041115027424</v>
       </c>
-      <c r="N3" s="43">
+      <c r="N3" s="37">
         <v>1.0572693640923954</v>
       </c>
     </row>
@@ -4566,31 +4904,31 @@
       <c r="E4" s="34">
         <v>2</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="37">
         <v>1.0634218497210675</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="37">
         <v>1.063557379006999</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="37">
         <v>1.0594135583132487</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="37">
         <v>1.1410529133725837</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="37">
         <v>1.0706972154367396</v>
       </c>
-      <c r="K4" s="43">
+      <c r="K4" s="37">
         <v>1.0658778360671342</v>
       </c>
-      <c r="L4" s="43">
+      <c r="L4" s="37">
         <v>1.0863088896010995</v>
       </c>
-      <c r="M4" s="43">
+      <c r="M4" s="37">
         <v>1.0827355347155851</v>
       </c>
-      <c r="N4" s="43">
+      <c r="N4" s="37">
         <v>1.0655072415642612</v>
       </c>
     </row>
@@ -4610,31 +4948,31 @@
       <c r="E5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="37">
         <v>1.1871057393021571</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="37">
         <v>1.1895030791292394</v>
       </c>
-      <c r="H5" s="43">
+      <c r="H5" s="37">
         <v>1.1564102497941353</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="37">
         <v>1.2710006900175661</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="37">
         <v>1.1597186442156466</v>
       </c>
-      <c r="K5" s="43">
+      <c r="K5" s="37">
         <v>1.2044227001564902</v>
       </c>
-      <c r="L5" s="43">
+      <c r="L5" s="37">
         <v>1.1867141492931483</v>
       </c>
-      <c r="M5" s="43">
+      <c r="M5" s="37">
         <v>1.1057317628900591</v>
       </c>
-      <c r="N5" s="43">
+      <c r="N5" s="37">
         <v>1.1385350925744731</v>
       </c>
     </row>
@@ -5105,4 +5443,1634 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C3208E-515B-4555-B380-473AA87B6645}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="44">
+        <v>1367247</v>
+      </c>
+      <c r="C4" s="44">
+        <v>930333</v>
+      </c>
+      <c r="D4" s="44">
+        <v>216621</v>
+      </c>
+      <c r="E4" s="44">
+        <v>114351</v>
+      </c>
+      <c r="F4" s="44">
+        <v>759882</v>
+      </c>
+      <c r="G4" s="44">
+        <v>625530</v>
+      </c>
+      <c r="H4" s="44">
+        <v>1558810</v>
+      </c>
+      <c r="I4" s="44">
+        <v>362423</v>
+      </c>
+      <c r="J4" s="44">
+        <v>407504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="44">
+        <v>922490</v>
+      </c>
+      <c r="C5" s="44">
+        <v>606479</v>
+      </c>
+      <c r="D5" s="44">
+        <v>137853</v>
+      </c>
+      <c r="E5" s="44">
+        <v>73823</v>
+      </c>
+      <c r="F5" s="44">
+        <v>540761</v>
+      </c>
+      <c r="G5" s="44">
+        <v>429564</v>
+      </c>
+      <c r="H5" s="44">
+        <v>1055954</v>
+      </c>
+      <c r="I5" s="44">
+        <v>229735</v>
+      </c>
+      <c r="J5" s="44">
+        <v>265533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="44">
+        <v>921061</v>
+      </c>
+      <c r="C6" s="44">
+        <v>605752</v>
+      </c>
+      <c r="D6" s="44">
+        <v>137710</v>
+      </c>
+      <c r="E6" s="44">
+        <v>73750</v>
+      </c>
+      <c r="F6" s="44">
+        <v>540475</v>
+      </c>
+      <c r="G6" s="44">
+        <v>429101</v>
+      </c>
+      <c r="H6" s="44">
+        <v>1054725</v>
+      </c>
+      <c r="I6" s="44">
+        <v>225581</v>
+      </c>
+      <c r="J6" s="44">
+        <v>264810</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="44">
+        <v>874563</v>
+      </c>
+      <c r="C7" s="44">
+        <v>570386</v>
+      </c>
+      <c r="D7" s="44">
+        <v>130613</v>
+      </c>
+      <c r="E7" s="44">
+        <v>70147</v>
+      </c>
+      <c r="F7" s="44">
+        <v>511902</v>
+      </c>
+      <c r="G7" s="44">
+        <v>409344</v>
+      </c>
+      <c r="H7" s="44">
+        <v>1007768</v>
+      </c>
+      <c r="I7" s="44">
+        <v>212151</v>
+      </c>
+      <c r="J7" s="44">
+        <v>251382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="44">
+        <v>46498</v>
+      </c>
+      <c r="C8" s="44">
+        <v>35366</v>
+      </c>
+      <c r="D8" s="44">
+        <v>7097</v>
+      </c>
+      <c r="E8" s="44">
+        <v>3603</v>
+      </c>
+      <c r="F8" s="44">
+        <v>28573</v>
+      </c>
+      <c r="G8" s="44">
+        <v>19757</v>
+      </c>
+      <c r="H8" s="44">
+        <v>46957</v>
+      </c>
+      <c r="I8" s="44">
+        <v>13430</v>
+      </c>
+      <c r="J8" s="44">
+        <v>13428</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="44">
+        <v>1429</v>
+      </c>
+      <c r="C9">
+        <v>727</v>
+      </c>
+      <c r="D9">
+        <v>143</v>
+      </c>
+      <c r="E9">
+        <v>73</v>
+      </c>
+      <c r="F9">
+        <v>286</v>
+      </c>
+      <c r="G9">
+        <v>463</v>
+      </c>
+      <c r="H9" s="44">
+        <v>1229</v>
+      </c>
+      <c r="I9" s="44">
+        <v>4154</v>
+      </c>
+      <c r="J9">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="44">
+        <v>444757</v>
+      </c>
+      <c r="C10" s="44">
+        <v>323854</v>
+      </c>
+      <c r="D10" s="44">
+        <v>78768</v>
+      </c>
+      <c r="E10" s="44">
+        <v>40528</v>
+      </c>
+      <c r="F10" s="44">
+        <v>219121</v>
+      </c>
+      <c r="G10" s="44">
+        <v>195966</v>
+      </c>
+      <c r="H10" s="44">
+        <v>502856</v>
+      </c>
+      <c r="I10" s="44">
+        <v>132688</v>
+      </c>
+      <c r="J10" s="44">
+        <v>141971</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="46">
+        <f>B7+B9</f>
+        <v>875992</v>
+      </c>
+      <c r="C11" s="46">
+        <f t="shared" ref="C11:J11" si="0">C7+C9</f>
+        <v>571113</v>
+      </c>
+      <c r="D11" s="46">
+        <f t="shared" si="0"/>
+        <v>130756</v>
+      </c>
+      <c r="E11" s="46">
+        <f t="shared" si="0"/>
+        <v>70220</v>
+      </c>
+      <c r="F11" s="46">
+        <f t="shared" si="0"/>
+        <v>512188</v>
+      </c>
+      <c r="G11" s="46">
+        <f t="shared" si="0"/>
+        <v>409807</v>
+      </c>
+      <c r="H11" s="46">
+        <f t="shared" si="0"/>
+        <v>1008997</v>
+      </c>
+      <c r="I11" s="46">
+        <f t="shared" si="0"/>
+        <v>216305</v>
+      </c>
+      <c r="J11" s="46">
+        <f t="shared" si="0"/>
+        <v>252105</v>
+      </c>
+      <c r="K11" s="44">
+        <f>SUM(B11:J11)</f>
+        <v>4047483</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E4CE5C-81B3-4E8A-8301-37F11CDAB451}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="44">
+        <v>1368100</v>
+      </c>
+      <c r="C4" s="44">
+        <v>926317</v>
+      </c>
+      <c r="D4" s="44">
+        <v>214016</v>
+      </c>
+      <c r="E4" s="44">
+        <v>113425</v>
+      </c>
+      <c r="F4" s="44">
+        <v>774619</v>
+      </c>
+      <c r="G4" s="44">
+        <v>630766</v>
+      </c>
+      <c r="H4" s="44">
+        <v>1556732</v>
+      </c>
+      <c r="I4" s="44">
+        <v>359609</v>
+      </c>
+      <c r="J4" s="44">
+        <v>411096</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="44">
+        <v>923970</v>
+      </c>
+      <c r="C5" s="44">
+        <v>601076</v>
+      </c>
+      <c r="D5" s="44">
+        <v>136409</v>
+      </c>
+      <c r="E5" s="44">
+        <v>71916</v>
+      </c>
+      <c r="F5" s="44">
+        <v>560066</v>
+      </c>
+      <c r="G5" s="44">
+        <v>433990</v>
+      </c>
+      <c r="H5" s="44">
+        <v>1059222</v>
+      </c>
+      <c r="I5" s="44">
+        <v>227911</v>
+      </c>
+      <c r="J5" s="44">
+        <v>268628</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="44">
+        <v>921454</v>
+      </c>
+      <c r="C6" s="44">
+        <v>601076</v>
+      </c>
+      <c r="D6" s="44">
+        <v>136401</v>
+      </c>
+      <c r="E6" s="44">
+        <v>71796</v>
+      </c>
+      <c r="F6" s="44">
+        <v>559900</v>
+      </c>
+      <c r="G6" s="44">
+        <v>433885</v>
+      </c>
+      <c r="H6" s="44">
+        <v>1057967</v>
+      </c>
+      <c r="I6" s="44">
+        <v>224509</v>
+      </c>
+      <c r="J6" s="44">
+        <v>268068</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="44">
+        <v>885937</v>
+      </c>
+      <c r="C7" s="44">
+        <v>576786</v>
+      </c>
+      <c r="D7" s="44">
+        <v>130860</v>
+      </c>
+      <c r="E7" s="44">
+        <v>69450</v>
+      </c>
+      <c r="F7" s="44">
+        <v>539057</v>
+      </c>
+      <c r="G7" s="44">
+        <v>421562</v>
+      </c>
+      <c r="H7" s="44">
+        <v>1021426</v>
+      </c>
+      <c r="I7" s="44">
+        <v>215481</v>
+      </c>
+      <c r="J7" s="44">
+        <v>258846</v>
+      </c>
+      <c r="K7" s="44">
+        <f t="shared" ref="K7:K10" si="0">SUM(B7:J7)</f>
+        <v>4119405</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="44">
+        <v>35517</v>
+      </c>
+      <c r="C8" s="44">
+        <v>24290</v>
+      </c>
+      <c r="D8" s="44">
+        <v>5541</v>
+      </c>
+      <c r="E8" s="44">
+        <v>2346</v>
+      </c>
+      <c r="F8" s="44">
+        <v>20843</v>
+      </c>
+      <c r="G8" s="44">
+        <v>12323</v>
+      </c>
+      <c r="H8" s="44">
+        <v>36541</v>
+      </c>
+      <c r="I8" s="44">
+        <v>9028</v>
+      </c>
+      <c r="J8" s="44">
+        <v>9222</v>
+      </c>
+      <c r="K8" s="44">
+        <f t="shared" si="0"/>
+        <v>155651</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="44">
+        <v>2516</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>120</v>
+      </c>
+      <c r="F9">
+        <v>166</v>
+      </c>
+      <c r="G9">
+        <v>105</v>
+      </c>
+      <c r="H9" s="44">
+        <v>1255</v>
+      </c>
+      <c r="I9" s="44">
+        <v>3402</v>
+      </c>
+      <c r="J9">
+        <v>560</v>
+      </c>
+      <c r="K9" s="44">
+        <f t="shared" si="0"/>
+        <v>8132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="44">
+        <v>444130</v>
+      </c>
+      <c r="C10" s="44">
+        <v>325241</v>
+      </c>
+      <c r="D10" s="44">
+        <v>77607</v>
+      </c>
+      <c r="E10" s="44">
+        <v>41509</v>
+      </c>
+      <c r="F10" s="44">
+        <v>214553</v>
+      </c>
+      <c r="G10" s="44">
+        <v>196776</v>
+      </c>
+      <c r="H10" s="44">
+        <v>497510</v>
+      </c>
+      <c r="I10" s="44">
+        <v>131698</v>
+      </c>
+      <c r="J10" s="44">
+        <v>142468</v>
+      </c>
+      <c r="K10" s="44">
+        <f t="shared" si="0"/>
+        <v>2071492</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="44">
+        <f>B7+B9</f>
+        <v>888453</v>
+      </c>
+      <c r="C11" s="44">
+        <f t="shared" ref="C11:J11" si="1">C7+C9</f>
+        <v>576786</v>
+      </c>
+      <c r="D11" s="44">
+        <f t="shared" si="1"/>
+        <v>130868</v>
+      </c>
+      <c r="E11" s="44">
+        <f t="shared" si="1"/>
+        <v>69570</v>
+      </c>
+      <c r="F11" s="44">
+        <f t="shared" si="1"/>
+        <v>539223</v>
+      </c>
+      <c r="G11" s="44">
+        <f t="shared" si="1"/>
+        <v>421667</v>
+      </c>
+      <c r="H11" s="44">
+        <f t="shared" si="1"/>
+        <v>1022681</v>
+      </c>
+      <c r="I11" s="44">
+        <f t="shared" si="1"/>
+        <v>218883</v>
+      </c>
+      <c r="J11" s="44">
+        <f t="shared" si="1"/>
+        <v>259406</v>
+      </c>
+      <c r="K11" s="44">
+        <f>SUM(B11:J11)</f>
+        <v>4127537</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F52BA6-CD06-4FAF-A0CB-FA0C0BE16874}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="44">
+        <v>1354894</v>
+      </c>
+      <c r="C4" s="44">
+        <v>935414</v>
+      </c>
+      <c r="D4" s="44">
+        <v>216956</v>
+      </c>
+      <c r="E4" s="44">
+        <v>113324</v>
+      </c>
+      <c r="F4" s="44">
+        <v>713617</v>
+      </c>
+      <c r="G4" s="44">
+        <v>609864</v>
+      </c>
+      <c r="H4" s="44">
+        <v>1535714</v>
+      </c>
+      <c r="I4" s="44">
+        <v>363577</v>
+      </c>
+      <c r="J4" s="44">
+        <v>403841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="44">
+        <v>899944</v>
+      </c>
+      <c r="C5" s="44">
+        <v>608978</v>
+      </c>
+      <c r="D5" s="44">
+        <v>135890</v>
+      </c>
+      <c r="E5" s="44">
+        <v>72423</v>
+      </c>
+      <c r="F5" s="44">
+        <v>489596</v>
+      </c>
+      <c r="G5" s="44">
+        <v>406948</v>
+      </c>
+      <c r="H5" s="44">
+        <v>1022939</v>
+      </c>
+      <c r="I5" s="44">
+        <v>226538</v>
+      </c>
+      <c r="J5" s="44">
+        <v>258482</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="44">
+        <v>898256</v>
+      </c>
+      <c r="C6" s="44">
+        <v>607564</v>
+      </c>
+      <c r="D6" s="44">
+        <v>135662</v>
+      </c>
+      <c r="E6" s="44">
+        <v>72423</v>
+      </c>
+      <c r="F6" s="44">
+        <v>489407</v>
+      </c>
+      <c r="G6" s="44">
+        <v>406915</v>
+      </c>
+      <c r="H6" s="44">
+        <v>1021919</v>
+      </c>
+      <c r="I6" s="44">
+        <v>221844</v>
+      </c>
+      <c r="J6" s="44">
+        <v>257891</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="44">
+        <v>838546</v>
+      </c>
+      <c r="C7" s="44">
+        <v>560979</v>
+      </c>
+      <c r="D7" s="44">
+        <v>125501</v>
+      </c>
+      <c r="E7" s="44">
+        <v>67802</v>
+      </c>
+      <c r="F7" s="44">
+        <v>448416</v>
+      </c>
+      <c r="G7" s="44">
+        <v>380381</v>
+      </c>
+      <c r="H7" s="44">
+        <v>960272</v>
+      </c>
+      <c r="I7" s="44">
+        <v>205695</v>
+      </c>
+      <c r="J7" s="44">
+        <v>240197</v>
+      </c>
+      <c r="K7" s="44">
+        <f t="shared" ref="K7:K10" si="0">SUM(B7:J7)</f>
+        <v>3827789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="44">
+        <v>59710</v>
+      </c>
+      <c r="C8" s="44">
+        <v>46585</v>
+      </c>
+      <c r="D8" s="44">
+        <v>10161</v>
+      </c>
+      <c r="E8" s="44">
+        <v>4621</v>
+      </c>
+      <c r="F8" s="44">
+        <v>40991</v>
+      </c>
+      <c r="G8" s="44">
+        <v>26534</v>
+      </c>
+      <c r="H8" s="44">
+        <v>61647</v>
+      </c>
+      <c r="I8" s="44">
+        <v>16149</v>
+      </c>
+      <c r="J8" s="44">
+        <v>17694</v>
+      </c>
+      <c r="K8" s="44">
+        <f t="shared" si="0"/>
+        <v>284092</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="44">
+        <v>1688</v>
+      </c>
+      <c r="C9" s="44">
+        <v>1414</v>
+      </c>
+      <c r="D9">
+        <v>228</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>189</v>
+      </c>
+      <c r="G9">
+        <v>33</v>
+      </c>
+      <c r="H9" s="44">
+        <v>1020</v>
+      </c>
+      <c r="I9" s="44">
+        <v>4694</v>
+      </c>
+      <c r="J9">
+        <v>591</v>
+      </c>
+      <c r="K9" s="44">
+        <f t="shared" si="0"/>
+        <v>9857</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="44">
+        <v>454950</v>
+      </c>
+      <c r="C10" s="44">
+        <v>326436</v>
+      </c>
+      <c r="D10" s="44">
+        <v>81066</v>
+      </c>
+      <c r="E10" s="44">
+        <v>40901</v>
+      </c>
+      <c r="F10" s="44">
+        <v>224021</v>
+      </c>
+      <c r="G10" s="44">
+        <v>202916</v>
+      </c>
+      <c r="H10" s="44">
+        <v>512775</v>
+      </c>
+      <c r="I10" s="44">
+        <v>137039</v>
+      </c>
+      <c r="J10" s="44">
+        <v>145359</v>
+      </c>
+      <c r="K10" s="44">
+        <f t="shared" si="0"/>
+        <v>2125463</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="44">
+        <f>B7+B9</f>
+        <v>840234</v>
+      </c>
+      <c r="C11" s="44">
+        <f t="shared" ref="C11:J11" si="1">C7+C9</f>
+        <v>562393</v>
+      </c>
+      <c r="D11" s="44">
+        <f t="shared" si="1"/>
+        <v>125729</v>
+      </c>
+      <c r="E11" s="44">
+        <f t="shared" si="1"/>
+        <v>67802</v>
+      </c>
+      <c r="F11" s="44">
+        <f t="shared" si="1"/>
+        <v>448605</v>
+      </c>
+      <c r="G11" s="44">
+        <f t="shared" si="1"/>
+        <v>380414</v>
+      </c>
+      <c r="H11" s="44">
+        <f t="shared" si="1"/>
+        <v>961292</v>
+      </c>
+      <c r="I11" s="44">
+        <f t="shared" si="1"/>
+        <v>210389</v>
+      </c>
+      <c r="J11" s="44">
+        <f t="shared" si="1"/>
+        <v>240788</v>
+      </c>
+      <c r="K11" s="44">
+        <f>SUM(B11:J11)</f>
+        <v>3837646</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C175EED6-C391-4CD1-9F97-C30AA63CF851}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="44">
+        <f>('ACS 2019 B23025'!B4+'ACS 2021 B23025'!B4)/2</f>
+        <v>1361497</v>
+      </c>
+      <c r="C4" s="44">
+        <f>('ACS 2019 B23025'!C4+'ACS 2021 B23025'!C4)/2</f>
+        <v>930865.5</v>
+      </c>
+      <c r="D4" s="44">
+        <f>('ACS 2019 B23025'!D4+'ACS 2021 B23025'!D4)/2</f>
+        <v>215486</v>
+      </c>
+      <c r="E4" s="44">
+        <f>('ACS 2019 B23025'!E4+'ACS 2021 B23025'!E4)/2</f>
+        <v>113374.5</v>
+      </c>
+      <c r="F4" s="44">
+        <f>('ACS 2019 B23025'!F4+'ACS 2021 B23025'!F4)/2</f>
+        <v>744118</v>
+      </c>
+      <c r="G4" s="44">
+        <f>('ACS 2019 B23025'!G4+'ACS 2021 B23025'!G4)/2</f>
+        <v>620315</v>
+      </c>
+      <c r="H4" s="44">
+        <f>('ACS 2019 B23025'!H4+'ACS 2021 B23025'!H4)/2</f>
+        <v>1546223</v>
+      </c>
+      <c r="I4" s="44">
+        <f>('ACS 2019 B23025'!I4+'ACS 2021 B23025'!I4)/2</f>
+        <v>361593</v>
+      </c>
+      <c r="J4" s="44">
+        <f>('ACS 2019 B23025'!J4+'ACS 2021 B23025'!J4)/2</f>
+        <v>407468.5</v>
+      </c>
+      <c r="K4" s="44">
+        <f>SUM(B4:J4)</f>
+        <v>6300940.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="44">
+        <f>('ACS 2019 B23025'!B5+'ACS 2021 B23025'!B5)/2</f>
+        <v>911957</v>
+      </c>
+      <c r="C5" s="44">
+        <f>('ACS 2019 B23025'!C5+'ACS 2021 B23025'!C5)/2</f>
+        <v>605027</v>
+      </c>
+      <c r="D5" s="44">
+        <f>('ACS 2019 B23025'!D5+'ACS 2021 B23025'!D5)/2</f>
+        <v>136149.5</v>
+      </c>
+      <c r="E5" s="44">
+        <f>('ACS 2019 B23025'!E5+'ACS 2021 B23025'!E5)/2</f>
+        <v>72169.5</v>
+      </c>
+      <c r="F5" s="44">
+        <f>('ACS 2019 B23025'!F5+'ACS 2021 B23025'!F5)/2</f>
+        <v>524831</v>
+      </c>
+      <c r="G5" s="44">
+        <f>('ACS 2019 B23025'!G5+'ACS 2021 B23025'!G5)/2</f>
+        <v>420469</v>
+      </c>
+      <c r="H5" s="44">
+        <f>('ACS 2019 B23025'!H5+'ACS 2021 B23025'!H5)/2</f>
+        <v>1041080.5</v>
+      </c>
+      <c r="I5" s="44">
+        <f>('ACS 2019 B23025'!I5+'ACS 2021 B23025'!I5)/2</f>
+        <v>227224.5</v>
+      </c>
+      <c r="J5" s="44">
+        <f>('ACS 2019 B23025'!J5+'ACS 2021 B23025'!J5)/2</f>
+        <v>263555</v>
+      </c>
+      <c r="K5" s="44">
+        <f t="shared" ref="K5:K11" si="0">SUM(B5:J5)</f>
+        <v>4202463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="44">
+        <f>('ACS 2019 B23025'!B6+'ACS 2021 B23025'!B6)/2</f>
+        <v>909855</v>
+      </c>
+      <c r="C6" s="44">
+        <f>('ACS 2019 B23025'!C6+'ACS 2021 B23025'!C6)/2</f>
+        <v>604320</v>
+      </c>
+      <c r="D6" s="44">
+        <f>('ACS 2019 B23025'!D6+'ACS 2021 B23025'!D6)/2</f>
+        <v>136031.5</v>
+      </c>
+      <c r="E6" s="44">
+        <f>('ACS 2019 B23025'!E6+'ACS 2021 B23025'!E6)/2</f>
+        <v>72109.5</v>
+      </c>
+      <c r="F6" s="44">
+        <f>('ACS 2019 B23025'!F6+'ACS 2021 B23025'!F6)/2</f>
+        <v>524653.5</v>
+      </c>
+      <c r="G6" s="44">
+        <f>('ACS 2019 B23025'!G6+'ACS 2021 B23025'!G6)/2</f>
+        <v>420400</v>
+      </c>
+      <c r="H6" s="44">
+        <f>('ACS 2019 B23025'!H6+'ACS 2021 B23025'!H6)/2</f>
+        <v>1039943</v>
+      </c>
+      <c r="I6" s="44">
+        <f>('ACS 2019 B23025'!I6+'ACS 2021 B23025'!I6)/2</f>
+        <v>223176.5</v>
+      </c>
+      <c r="J6" s="44">
+        <f>('ACS 2019 B23025'!J6+'ACS 2021 B23025'!J6)/2</f>
+        <v>262979.5</v>
+      </c>
+      <c r="K6" s="44">
+        <f t="shared" si="0"/>
+        <v>4193468.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="44">
+        <f>('ACS 2019 B23025'!B7+'ACS 2021 B23025'!B7)/2</f>
+        <v>862241.5</v>
+      </c>
+      <c r="C7" s="44">
+        <f>('ACS 2019 B23025'!C7+'ACS 2021 B23025'!C7)/2</f>
+        <v>568882.5</v>
+      </c>
+      <c r="D7" s="44">
+        <f>('ACS 2019 B23025'!D7+'ACS 2021 B23025'!D7)/2</f>
+        <v>128180.5</v>
+      </c>
+      <c r="E7" s="44">
+        <f>('ACS 2019 B23025'!E7+'ACS 2021 B23025'!E7)/2</f>
+        <v>68626</v>
+      </c>
+      <c r="F7" s="44">
+        <f>('ACS 2019 B23025'!F7+'ACS 2021 B23025'!F7)/2</f>
+        <v>493736.5</v>
+      </c>
+      <c r="G7" s="44">
+        <f>('ACS 2019 B23025'!G7+'ACS 2021 B23025'!G7)/2</f>
+        <v>400971.5</v>
+      </c>
+      <c r="H7" s="44">
+        <f>('ACS 2019 B23025'!H7+'ACS 2021 B23025'!H7)/2</f>
+        <v>990849</v>
+      </c>
+      <c r="I7" s="44">
+        <f>('ACS 2019 B23025'!I7+'ACS 2021 B23025'!I7)/2</f>
+        <v>210588</v>
+      </c>
+      <c r="J7" s="44">
+        <f>('ACS 2019 B23025'!J7+'ACS 2021 B23025'!J7)/2</f>
+        <v>249521.5</v>
+      </c>
+      <c r="K7" s="44">
+        <f t="shared" si="0"/>
+        <v>3973597</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="44">
+        <f>('ACS 2019 B23025'!B8+'ACS 2021 B23025'!B8)/2</f>
+        <v>47613.5</v>
+      </c>
+      <c r="C8" s="44">
+        <f>('ACS 2019 B23025'!C8+'ACS 2021 B23025'!C8)/2</f>
+        <v>35437.5</v>
+      </c>
+      <c r="D8" s="44">
+        <f>('ACS 2019 B23025'!D8+'ACS 2021 B23025'!D8)/2</f>
+        <v>7851</v>
+      </c>
+      <c r="E8" s="44">
+        <f>('ACS 2019 B23025'!E8+'ACS 2021 B23025'!E8)/2</f>
+        <v>3483.5</v>
+      </c>
+      <c r="F8" s="44">
+        <f>('ACS 2019 B23025'!F8+'ACS 2021 B23025'!F8)/2</f>
+        <v>30917</v>
+      </c>
+      <c r="G8" s="44">
+        <f>('ACS 2019 B23025'!G8+'ACS 2021 B23025'!G8)/2</f>
+        <v>19428.5</v>
+      </c>
+      <c r="H8" s="44">
+        <f>('ACS 2019 B23025'!H8+'ACS 2021 B23025'!H8)/2</f>
+        <v>49094</v>
+      </c>
+      <c r="I8" s="44">
+        <f>('ACS 2019 B23025'!I8+'ACS 2021 B23025'!I8)/2</f>
+        <v>12588.5</v>
+      </c>
+      <c r="J8" s="44">
+        <f>('ACS 2019 B23025'!J8+'ACS 2021 B23025'!J8)/2</f>
+        <v>13458</v>
+      </c>
+      <c r="K8" s="44">
+        <f t="shared" si="0"/>
+        <v>219871.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="44">
+        <f>('ACS 2019 B23025'!B9+'ACS 2021 B23025'!B9)/2</f>
+        <v>2102</v>
+      </c>
+      <c r="C9" s="44">
+        <f>('ACS 2019 B23025'!C9+'ACS 2021 B23025'!C9)/2</f>
+        <v>707</v>
+      </c>
+      <c r="D9" s="44">
+        <f>('ACS 2019 B23025'!D9+'ACS 2021 B23025'!D9)/2</f>
+        <v>118</v>
+      </c>
+      <c r="E9" s="44">
+        <f>('ACS 2019 B23025'!E9+'ACS 2021 B23025'!E9)/2</f>
+        <v>60</v>
+      </c>
+      <c r="F9" s="44">
+        <f>('ACS 2019 B23025'!F9+'ACS 2021 B23025'!F9)/2</f>
+        <v>177.5</v>
+      </c>
+      <c r="G9" s="44">
+        <f>('ACS 2019 B23025'!G9+'ACS 2021 B23025'!G9)/2</f>
+        <v>69</v>
+      </c>
+      <c r="H9" s="44">
+        <f>('ACS 2019 B23025'!H9+'ACS 2021 B23025'!H9)/2</f>
+        <v>1137.5</v>
+      </c>
+      <c r="I9" s="44">
+        <f>('ACS 2019 B23025'!I9+'ACS 2021 B23025'!I9)/2</f>
+        <v>4048</v>
+      </c>
+      <c r="J9" s="44">
+        <f>('ACS 2019 B23025'!J9+'ACS 2021 B23025'!J9)/2</f>
+        <v>575.5</v>
+      </c>
+      <c r="K9" s="44">
+        <f t="shared" si="0"/>
+        <v>8994.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="44">
+        <f>('ACS 2019 B23025'!B10+'ACS 2021 B23025'!B10)/2</f>
+        <v>449540</v>
+      </c>
+      <c r="C10" s="44">
+        <f>('ACS 2019 B23025'!C10+'ACS 2021 B23025'!C10)/2</f>
+        <v>325838.5</v>
+      </c>
+      <c r="D10" s="44">
+        <f>('ACS 2019 B23025'!D10+'ACS 2021 B23025'!D10)/2</f>
+        <v>79336.5</v>
+      </c>
+      <c r="E10" s="44">
+        <f>('ACS 2019 B23025'!E10+'ACS 2021 B23025'!E10)/2</f>
+        <v>41205</v>
+      </c>
+      <c r="F10" s="44">
+        <f>('ACS 2019 B23025'!F10+'ACS 2021 B23025'!F10)/2</f>
+        <v>219287</v>
+      </c>
+      <c r="G10" s="44">
+        <f>('ACS 2019 B23025'!G10+'ACS 2021 B23025'!G10)/2</f>
+        <v>199846</v>
+      </c>
+      <c r="H10" s="44">
+        <f>('ACS 2019 B23025'!H10+'ACS 2021 B23025'!H10)/2</f>
+        <v>505142.5</v>
+      </c>
+      <c r="I10" s="44">
+        <f>('ACS 2019 B23025'!I10+'ACS 2021 B23025'!I10)/2</f>
+        <v>134368.5</v>
+      </c>
+      <c r="J10" s="44">
+        <f>('ACS 2019 B23025'!J10+'ACS 2021 B23025'!J10)/2</f>
+        <v>143913.5</v>
+      </c>
+      <c r="K10" s="44">
+        <f t="shared" si="0"/>
+        <v>2098477.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="44">
+        <f>('ACS 2019 B23025'!B11+'ACS 2021 B23025'!B11)/2</f>
+        <v>864343.5</v>
+      </c>
+      <c r="C11" s="44">
+        <f>('ACS 2019 B23025'!C11+'ACS 2021 B23025'!C11)/2</f>
+        <v>569589.5</v>
+      </c>
+      <c r="D11" s="44">
+        <f>('ACS 2019 B23025'!D11+'ACS 2021 B23025'!D11)/2</f>
+        <v>128298.5</v>
+      </c>
+      <c r="E11" s="44">
+        <f>('ACS 2019 B23025'!E11+'ACS 2021 B23025'!E11)/2</f>
+        <v>68686</v>
+      </c>
+      <c r="F11" s="44">
+        <f>('ACS 2019 B23025'!F11+'ACS 2021 B23025'!F11)/2</f>
+        <v>493914</v>
+      </c>
+      <c r="G11" s="44">
+        <f>('ACS 2019 B23025'!G11+'ACS 2021 B23025'!G11)/2</f>
+        <v>401040.5</v>
+      </c>
+      <c r="H11" s="44">
+        <f>('ACS 2019 B23025'!H11+'ACS 2021 B23025'!H11)/2</f>
+        <v>991986.5</v>
+      </c>
+      <c r="I11" s="44">
+        <f>('ACS 2019 B23025'!I11+'ACS 2021 B23025'!I11)/2</f>
+        <v>214636</v>
+      </c>
+      <c r="J11" s="44">
+        <f>('ACS 2019 B23025'!J11+'ACS 2021 B23025'!J11)/2</f>
+        <v>250097</v>
+      </c>
+      <c r="K11" s="44">
+        <f t="shared" si="0"/>
+        <v>3982591.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35BA19A-2396-4E69-86B5-4D0B28D105F5}">
+  <dimension ref="A2:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="44">
+        <v>864343.5</v>
+      </c>
+      <c r="C6" s="44">
+        <v>875992</v>
+      </c>
+      <c r="D6" s="48">
+        <v>0.98670250413245786</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="44">
+        <v>569589.5</v>
+      </c>
+      <c r="C7" s="44">
+        <v>571113</v>
+      </c>
+      <c r="D7" s="48">
+        <v>0.99733240181890448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="44">
+        <v>128298.5</v>
+      </c>
+      <c r="C8" s="44">
+        <v>130756</v>
+      </c>
+      <c r="D8" s="48">
+        <v>0.98120545137508031</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="44">
+        <v>68686</v>
+      </c>
+      <c r="C9" s="44">
+        <v>70220</v>
+      </c>
+      <c r="D9" s="48">
+        <v>0.97815437197379662</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="44">
+        <v>493914</v>
+      </c>
+      <c r="C10" s="44">
+        <v>512188</v>
+      </c>
+      <c r="D10" s="48">
+        <v>0.96432169437784565</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="44">
+        <v>401040.5</v>
+      </c>
+      <c r="C11" s="44">
+        <v>409807</v>
+      </c>
+      <c r="D11" s="48">
+        <v>0.97860822289516769</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="44">
+        <v>991986.5</v>
+      </c>
+      <c r="C12" s="44">
+        <v>1008997</v>
+      </c>
+      <c r="D12" s="48">
+        <v>0.98314117881420859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="44">
+        <v>214636</v>
+      </c>
+      <c r="C13" s="44">
+        <v>216305</v>
+      </c>
+      <c r="D13" s="48">
+        <v>0.99228404336469334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="44">
+        <v>250097</v>
+      </c>
+      <c r="C14" s="44">
+        <v>252105</v>
+      </c>
+      <c r="D14" s="48">
+        <v>0.99203506475476488</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="44">
+        <v>3982591.5</v>
+      </c>
+      <c r="C15" s="44">
+        <v>4047483</v>
+      </c>
+      <c r="D15" s="48">
+        <v>0.98396744347042342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>